<commit_message>
Change inserting date from manually to grab it from website automatically
</commit_message>
<xml_diff>
--- a/data/Industry-Indices.xlsx
+++ b/data/Industry-Indices.xlsx
@@ -411,12 +411,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -430,27 +430,27 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>7650169488000000</v>
+        <v>7650169488</v>
       </c>
       <c r="F2" t="n">
         <v>236046</v>
       </c>
       <c r="G2" t="n">
-        <v>2740000000</v>
+        <v>2740</v>
       </c>
       <c r="H2" t="n">
-        <v>10212891000000</v>
+        <v>10212891</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -464,27 +464,27 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>269025262000000</v>
+        <v>269025262</v>
       </c>
       <c r="F3" t="n">
         <v>62425</v>
       </c>
       <c r="G3" t="n">
-        <v>1399000000</v>
+        <v>1399</v>
       </c>
       <c r="H3" t="n">
-        <v>2610194000000</v>
+        <v>2610194</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -498,27 +498,27 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>644373421000000</v>
+        <v>644373421</v>
       </c>
       <c r="F4" t="n">
         <v>50274</v>
       </c>
       <c r="G4" t="n">
-        <v>1447000000</v>
+        <v>1447</v>
       </c>
       <c r="H4" t="n">
-        <v>1194232000000</v>
+        <v>1194232</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -532,27 +532,29 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1900527339000000</v>
+        <v>1900527339</v>
       </c>
       <c r="F5" t="n">
         <v>20390</v>
       </c>
-      <c r="G5" t="n">
-        <v>172604000</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">172.604 </t>
+        </is>
       </c>
       <c r="H5" t="n">
-        <v>989110000000</v>
+        <v>989110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -566,27 +568,29 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1389537365000000</v>
+        <v>1389537365</v>
       </c>
       <c r="F6" t="n">
         <v>15898</v>
       </c>
-      <c r="G6" t="n">
-        <v>112454000</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">112.454 </t>
+        </is>
       </c>
       <c r="H6" t="n">
-        <v>729291000000</v>
+        <v>729291</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -600,27 +604,29 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>327414867000000</v>
+        <v>327414867</v>
       </c>
       <c r="F7" t="n">
         <v>15010</v>
       </c>
-      <c r="G7" t="n">
-        <v>90188000</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">90.188 </t>
+        </is>
       </c>
       <c r="H7" t="n">
-        <v>619402000000</v>
+        <v>619402</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -634,27 +640,29 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>132475867000000</v>
+        <v>132475867</v>
       </c>
       <c r="F8" t="n">
         <v>16479</v>
       </c>
-      <c r="G8" t="n">
-        <v>141383000</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">141.383 </t>
+        </is>
       </c>
       <c r="H8" t="n">
-        <v>602031000000</v>
+        <v>602031</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -668,27 +676,29 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>152416614000000</v>
+        <v>152416614</v>
       </c>
       <c r="F9" t="n">
         <v>19931</v>
       </c>
-      <c r="G9" t="n">
-        <v>298003000</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">298.003 </t>
+        </is>
       </c>
       <c r="H9" t="n">
-        <v>579976000000</v>
+        <v>579976</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -702,27 +712,29 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>234634329000000</v>
+        <v>234634329</v>
       </c>
       <c r="F10" t="n">
         <v>10125</v>
       </c>
-      <c r="G10" t="n">
-        <v>127488000</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">127.488 </t>
+        </is>
       </c>
       <c r="H10" t="n">
-        <v>551518000000</v>
+        <v>551518</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -736,27 +748,29 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>244839872000000</v>
+        <v>244839872</v>
       </c>
       <c r="F11" t="n">
         <v>2738</v>
       </c>
-      <c r="G11" t="n">
-        <v>42805000</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">42.805 </t>
+        </is>
       </c>
       <c r="H11" t="n">
-        <v>513549000000</v>
+        <v>513549</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -770,27 +784,29 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>796835303000000</v>
+        <v>796835303</v>
       </c>
       <c r="F12" t="n">
         <v>10137</v>
       </c>
-      <c r="G12" t="n">
-        <v>32724000</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">32.724 </t>
+        </is>
       </c>
       <c r="H12" t="n">
-        <v>436921000000</v>
+        <v>436921</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -804,27 +820,29 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>58769609000000</v>
+        <v>58769609</v>
       </c>
       <c r="F13" t="n">
         <v>5850</v>
       </c>
-      <c r="G13" t="n">
-        <v>41629000</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">41.629 </t>
+        </is>
       </c>
       <c r="H13" t="n">
-        <v>404823000000</v>
+        <v>404823</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -838,27 +856,29 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>39352522000000</v>
+        <v>39352522</v>
       </c>
       <c r="F14" t="n">
         <v>9250</v>
       </c>
-      <c r="G14" t="n">
-        <v>40843000</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">40.843 </t>
+        </is>
       </c>
       <c r="H14" t="n">
-        <v>336782000000</v>
+        <v>336782</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -872,27 +892,29 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>761443842000000</v>
+        <v>761443842</v>
       </c>
       <c r="F15" t="n">
         <v>11983</v>
       </c>
-      <c r="G15" t="n">
-        <v>70270000</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">70.270 </t>
+        </is>
       </c>
       <c r="H15" t="n">
-        <v>328300000000</v>
+        <v>328300</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -906,27 +928,29 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>22727610000000</v>
+        <v>22727610</v>
       </c>
       <c r="F16" t="n">
         <v>8676</v>
       </c>
-      <c r="G16" t="n">
-        <v>168368000</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">168.368 </t>
+        </is>
       </c>
       <c r="H16" t="n">
-        <v>271096000000</v>
+        <v>271096</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -940,27 +964,29 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>95823366000000</v>
+        <v>95823366</v>
       </c>
       <c r="F17" t="n">
         <v>4472</v>
       </c>
-      <c r="G17" t="n">
-        <v>36102000</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">36.102 </t>
+        </is>
       </c>
       <c r="H17" t="n">
-        <v>237861000000</v>
+        <v>237861</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -974,27 +1000,29 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>58429483000000</v>
+        <v>58429483</v>
       </c>
       <c r="F18" t="n">
         <v>6272</v>
       </c>
-      <c r="G18" t="n">
-        <v>37891000</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">37.891 </t>
+        </is>
       </c>
       <c r="H18" t="n">
-        <v>231235000000</v>
+        <v>231235</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1008,27 +1036,29 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>437081000000000</v>
+        <v>437081000</v>
       </c>
       <c r="F19" t="n">
         <v>3757</v>
       </c>
-      <c r="G19" t="n">
-        <v>68575000</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">68.575 </t>
+        </is>
       </c>
       <c r="H19" t="n">
-        <v>200216000000</v>
+        <v>200216</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1042,27 +1072,29 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>43630457000000</v>
+        <v>43630457</v>
       </c>
       <c r="F20" t="n">
         <v>6455</v>
       </c>
-      <c r="G20" t="n">
-        <v>88702000</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">88.702 </t>
+        </is>
       </c>
       <c r="H20" t="n">
-        <v>163857000000</v>
+        <v>163857</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1076,27 +1108,29 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>165223800000000</v>
+        <v>165223800</v>
       </c>
       <c r="F21" t="n">
         <v>2758</v>
       </c>
-      <c r="G21" t="n">
-        <v>24869000</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">24.869 </t>
+        </is>
       </c>
       <c r="H21" t="n">
-        <v>158853000000</v>
+        <v>158853</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1110,27 +1144,29 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>25372000000000</v>
+        <v>25372000</v>
       </c>
       <c r="F22" t="n">
         <v>2063</v>
       </c>
-      <c r="G22" t="n">
-        <v>24196000</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">24.196 </t>
+        </is>
       </c>
       <c r="H22" t="n">
-        <v>153477000000</v>
+        <v>153477</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1144,27 +1180,29 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>33797691000000</v>
+        <v>33797691</v>
       </c>
       <c r="F23" t="n">
         <v>3553</v>
       </c>
-      <c r="G23" t="n">
-        <v>21118000</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">21.118 </t>
+        </is>
       </c>
       <c r="H23" t="n">
-        <v>152628000000</v>
+        <v>152628</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1178,27 +1216,29 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>29702528000000</v>
+        <v>29702528</v>
       </c>
       <c r="F24" t="n">
         <v>4777</v>
       </c>
-      <c r="G24" t="n">
-        <v>56331000</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">56.331 </t>
+        </is>
       </c>
       <c r="H24" t="n">
-        <v>150879000000</v>
+        <v>150879</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1212,27 +1252,29 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>96448191000000</v>
+        <v>96448191</v>
       </c>
       <c r="F25" t="n">
         <v>5880</v>
       </c>
-      <c r="G25" t="n">
-        <v>38844000</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">38.844 </t>
+        </is>
       </c>
       <c r="H25" t="n">
-        <v>141262000000</v>
+        <v>141262</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1246,27 +1288,29 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>40033876000000</v>
+        <v>40033876</v>
       </c>
       <c r="F26" t="n">
         <v>4669</v>
       </c>
-      <c r="G26" t="n">
-        <v>12820000</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12.820 </t>
+        </is>
       </c>
       <c r="H26" t="n">
-        <v>139909000000</v>
+        <v>139909</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1280,27 +1324,29 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>36108800000000</v>
+        <v>36108800</v>
       </c>
       <c r="F27" t="n">
         <v>2991</v>
       </c>
-      <c r="G27" t="n">
-        <v>47100000</v>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">47.100 </t>
+        </is>
       </c>
       <c r="H27" t="n">
-        <v>104581000000</v>
+        <v>104581</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1314,27 +1360,29 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>11616352000000</v>
+        <v>11616352</v>
       </c>
       <c r="F28" t="n">
         <v>2535</v>
       </c>
-      <c r="G28" t="n">
-        <v>18037000</v>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">18.037 </t>
+        </is>
       </c>
       <c r="H28" t="n">
-        <v>77872000000</v>
+        <v>77872</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1348,27 +1396,29 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>76231900000000</v>
+        <v>76231900</v>
       </c>
       <c r="F29" t="n">
         <v>2975</v>
       </c>
-      <c r="G29" t="n">
-        <v>12208000</v>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12.208 </t>
+        </is>
       </c>
       <c r="H29" t="n">
-        <v>69444000000</v>
+        <v>69444</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1382,27 +1432,29 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>334939200000000</v>
+        <v>334939200</v>
       </c>
       <c r="F30" t="n">
         <v>2216</v>
       </c>
-      <c r="G30" t="n">
-        <v>27713000</v>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">27.713 </t>
+        </is>
       </c>
       <c r="H30" t="n">
-        <v>67117000000.00001</v>
+        <v>67117</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1416,27 +1468,29 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>19399846000000</v>
+        <v>19399846</v>
       </c>
       <c r="F31" t="n">
         <v>1230</v>
       </c>
-      <c r="G31" t="n">
-        <v>12571000</v>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12.571 </t>
+        </is>
       </c>
       <c r="H31" t="n">
-        <v>46808000000</v>
+        <v>46808</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1450,27 +1504,29 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>6219562000000</v>
+        <v>6219562</v>
       </c>
       <c r="F32" t="n">
         <v>1317</v>
       </c>
-      <c r="G32" t="n">
-        <v>4050000</v>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4.050 </t>
+        </is>
       </c>
       <c r="H32" t="n">
-        <v>41133000000</v>
+        <v>41133</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1484,27 +1540,29 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>7747230000000</v>
+        <v>7747230</v>
       </c>
       <c r="F33" t="n">
         <v>657</v>
       </c>
-      <c r="G33" t="n">
-        <v>3840000</v>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3.840 </t>
+        </is>
       </c>
       <c r="H33" t="n">
-        <v>33343000000</v>
+        <v>33343</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1518,27 +1576,29 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>2114180000000</v>
+        <v>2114180</v>
       </c>
       <c r="F34" t="n">
         <v>639</v>
       </c>
-      <c r="G34" t="n">
-        <v>2203000</v>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2.203 </t>
+        </is>
       </c>
       <c r="H34" t="n">
-        <v>25174000000</v>
+        <v>25174</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1552,7 +1612,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>41123000000000</v>
+        <v>41123000</v>
       </c>
       <c r="F35" t="n">
         <v>929</v>
@@ -1561,18 +1621,18 @@
         <v>561815</v>
       </c>
       <c r="H35" t="n">
-        <v>23104000000</v>
+        <v>23104</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1586,27 +1646,29 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>1254852000000</v>
+        <v>1254852</v>
       </c>
       <c r="F36" t="n">
         <v>789</v>
       </c>
-      <c r="G36" t="n">
-        <v>2381000</v>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2.381 </t>
+        </is>
       </c>
       <c r="H36" t="n">
-        <v>18445000000</v>
+        <v>18445</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1620,27 +1682,29 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>7046820000000</v>
+        <v>7046820</v>
       </c>
       <c r="F37" t="n">
         <v>299</v>
       </c>
-      <c r="G37" t="n">
-        <v>1906000</v>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1.906 </t>
+        </is>
       </c>
       <c r="H37" t="n">
-        <v>13567000000</v>
+        <v>13567</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1654,7 +1718,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>3223500000000</v>
+        <v>3223500</v>
       </c>
       <c r="F38" t="n">
         <v>168</v>
@@ -1663,18 +1727,18 @@
         <v>645886</v>
       </c>
       <c r="H38" t="n">
-        <v>6940000000</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1688,7 +1752,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2614576000000</v>
+        <v>2614576</v>
       </c>
       <c r="F39" t="n">
         <v>145</v>
@@ -1697,18 +1761,18 @@
         <v>97867</v>
       </c>
       <c r="H39" t="n">
-        <v>1576000000</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1722,7 +1786,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>3405027000000</v>
+        <v>3405027</v>
       </c>
       <c r="F40" t="n">
         <v>76</v>
@@ -1731,18 +1795,18 @@
         <v>555894</v>
       </c>
       <c r="H40" t="n">
-        <v>1405000000</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1756,7 +1820,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>4561074000000</v>
+        <v>4561074</v>
       </c>
       <c r="F41" t="n">
         <v>5</v>
@@ -1764,19 +1828,21 @@
       <c r="G41" t="n">
         <v>25209</v>
       </c>
-      <c r="H41" t="n">
-        <v>481920000</v>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">481.920 </t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20190603</t>
+          <t>2019-06-03</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>13980313</t>
+          <t>1398-03-13</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1790,7 +1856,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>9313400000000</v>
+        <v>9313400</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>

</xml_diff>